<commit_message>
generate named range only if autoflter applied
</commit_message>
<xml_diff>
--- a/test/out/autofilter.xlsx
+++ b/test/out/autofilter.xlsx
@@ -7,12 +7,12 @@
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="NEURO RAD" sheetId="1" r:id="rId1"/>
+    <sheet name="NEURO ONC" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" hidden="1" localSheetId="0">'sheet1'!$A$1:$J$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" hidden="1" localSheetId="1">'sheet2'!$A$1:$J$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" hidden="1" localSheetId="0">'NEURO RAD'!$A$1:$J$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" hidden="1" localSheetId="1">'NEURO ONC'!$A$1:$J$12</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>

</xml_diff>